<commit_message>
new version 2024-5-31 add script for do some daily work
</commit_message>
<xml_diff>
--- a/AxleHireToolsGUI/utils/files/dictionary.xlsx
+++ b/AxleHireToolsGUI/utils/files/dictionary.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE22FBA-74E0-451C-A244-1619F4002F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F995AE1-FE6D-4564-A1B1-98635D1ADB9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="118">
   <si>
     <t>Operation</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Wrong address</t>
   </si>
   <si>
-    <t>Package refused</t>
-  </si>
-  <si>
     <t>Cancelled Order</t>
   </si>
   <si>
@@ -116,24 +113,9 @@
     <t>Outside Service Area</t>
   </si>
   <si>
-    <t>pickup ok but delivery failed - redeliver requested</t>
-  </si>
-  <si>
     <t>Rescheduled</t>
   </si>
   <si>
-    <t>Inbound late</t>
-  </si>
-  <si>
-    <t>Received late</t>
-  </si>
-  <si>
-    <t>Received missing</t>
-  </si>
-  <si>
-    <t>Received damaged</t>
-  </si>
-  <si>
     <t>Routing</t>
   </si>
   <si>
@@ -191,24 +173,6 @@
     <t>Not Delivered</t>
   </si>
   <si>
-    <t>pickup ok but delivery failed - out of chain</t>
-  </si>
-  <si>
-    <t>Not delivered</t>
-  </si>
-  <si>
-    <t>pickup ok but delivery failed</t>
-  </si>
-  <si>
-    <t>pickup ok but delivery failed - pending</t>
-  </si>
-  <si>
-    <t>pickup ok but delivery failed - missing</t>
-  </si>
-  <si>
-    <t>pickup ok but delivery failed - discarded</t>
-  </si>
-  <si>
     <t>Driver didn't follow instruction</t>
   </si>
   <si>
@@ -221,19 +185,7 @@
     <t>Delivered to Wrong Address</t>
   </si>
   <si>
-    <t>Pickup after 12pm but delivery late for same day</t>
-  </si>
-  <si>
     <t>Late</t>
-  </si>
-  <si>
-    <t>pickup late for 1 day and delivery late for 1 day</t>
-  </si>
-  <si>
-    <t>pickup ok but delivery late for same day</t>
-  </si>
-  <si>
-    <t>pickup ok but delivery late for 1 day</t>
   </si>
   <si>
     <t>Issue Category</t>
@@ -404,25 +356,82 @@
     <t>Package not received by AxleHire</t>
   </si>
   <si>
-    <t>Inbound missing</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Inbound damaged</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>AX linehaul issue</t>
-  </si>
-  <si>
-    <t>AX linehaul late</t>
   </si>
   <si>
     <t>Out of delivery area</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>pickup ok but delivery late for same day</t>
+    <t>Pickup ok but delivery late for 1 day</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pickup ok but delivery late for same day</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pickup after 12pm but delivery late for same day</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pickup late for 1 day and delivery late for 1 day</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pickup ok but delivery failed - out of chain</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pickup ok but delivery failed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pickup ok but delivery failed - pending</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pickup ok but delivery failed - missing</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pickup ok but delivery failed - discarded</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AX linehaul late</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inbound Damaged</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inbound Missing</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inbound Late</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pickup ok but delivery failed - redeliver requested</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Received Late</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Received Missing</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Received Damaged</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package Refused</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -566,7 +575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -588,7 +597,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -874,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="E120" sqref="E120"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -890,22 +898,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="14.5">
       <c r="B1" s="9" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.5">
@@ -923,8 +931,8 @@
       <c r="F2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="17" t="s">
-        <v>112</v>
+      <c r="G2" s="16" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18.5">
@@ -942,8 +950,8 @@
       <c r="F3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="17" t="s">
-        <v>112</v>
+      <c r="G3" s="16" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18.5">
@@ -961,8 +969,8 @@
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="17" t="s">
-        <v>112</v>
+      <c r="G4" s="16" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18.5">
@@ -980,8 +988,8 @@
       <c r="F5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="17" t="s">
-        <v>112</v>
+      <c r="G5" s="16" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18.5">
@@ -999,8 +1007,8 @@
       <c r="F6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="17" t="s">
-        <v>112</v>
+      <c r="G6" s="16" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.5">
@@ -1018,8 +1026,8 @@
       <c r="F7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="17" t="s">
-        <v>112</v>
+      <c r="G7" s="16" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="14.5">
@@ -1241,10 +1249,10 @@
         <v>17</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>25</v>
+        <v>117</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>25</v>
+        <v>117</v>
       </c>
       <c r="G21" s="8"/>
     </row>
@@ -1258,10 +1266,10 @@
         <v>17</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G22" s="8"/>
     </row>
@@ -1275,10 +1283,10 @@
         <v>17</v>
       </c>
       <c r="E23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="13" t="s">
         <v>27</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>28</v>
       </c>
       <c r="G23" s="8"/>
     </row>
@@ -1292,10 +1300,10 @@
         <v>17</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G24" s="8"/>
     </row>
@@ -1309,10 +1317,10 @@
         <v>17</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>29</v>
+        <v>113</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G25" s="8"/>
     </row>
@@ -1326,10 +1334,10 @@
         <v>17</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>31</v>
+        <v>112</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>32</v>
+        <v>114</v>
       </c>
       <c r="G26" s="8"/>
     </row>
@@ -1343,10 +1351,10 @@
         <v>17</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>33</v>
+        <v>115</v>
       </c>
       <c r="G27" s="8"/>
     </row>
@@ -1360,10 +1368,10 @@
         <v>17</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>34</v>
+        <v>116</v>
       </c>
       <c r="G28" s="8"/>
     </row>
@@ -1377,10 +1385,10 @@
         <v>17</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="G29" s="8"/>
     </row>
@@ -1391,13 +1399,13 @@
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="4" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G30" s="8"/>
     </row>
@@ -1408,13 +1416,13 @@
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G31" s="8"/>
     </row>
@@ -1439,13 +1447,13 @@
         <v>0</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G33" s="18" t="s">
-        <v>111</v>
+        <v>33</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="18.5">
@@ -1458,13 +1466,13 @@
         <v>0</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="G34" s="18" t="s">
-        <v>111</v>
+        <v>35</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="18.5">
@@ -1477,13 +1485,13 @@
         <v>0</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G35" s="18" t="s">
-        <v>111</v>
+        <v>33</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="18.5">
@@ -1499,10 +1507,10 @@
         <v>9</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G36" s="18" t="s">
-        <v>111</v>
+        <v>33</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="18.5">
@@ -1518,10 +1526,10 @@
         <v>7</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G37" s="18" t="s">
-        <v>111</v>
+        <v>33</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="18.5">
@@ -1534,13 +1542,13 @@
         <v>0</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G38" s="18" t="s">
-        <v>111</v>
+        <v>33</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="18.5">
@@ -1553,13 +1561,13 @@
         <v>0</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G39" s="18" t="s">
-        <v>111</v>
+        <v>33</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="18.5">
@@ -1572,13 +1580,13 @@
         <v>0</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G40" s="18" t="s">
-        <v>111</v>
+        <v>33</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="18.5">
@@ -1594,10 +1602,10 @@
         <v>3</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G41" s="18" t="s">
-        <v>111</v>
+        <v>33</v>
+      </c>
+      <c r="G41" s="17" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="18.5">
@@ -1610,13 +1618,13 @@
         <v>0</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F42" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G42" s="18" t="s">
-        <v>111</v>
+        <v>33</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="18.5">
@@ -1632,10 +1640,10 @@
         <v>1</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G43" s="18" t="s">
-        <v>111</v>
+        <v>33</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="18.5">
@@ -1651,10 +1659,10 @@
         <v>3</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G44" s="18" t="s">
-        <v>111</v>
+        <v>33</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="18.5">
@@ -1670,10 +1678,10 @@
         <v>4</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G45" s="18" t="s">
-        <v>111</v>
+        <v>33</v>
+      </c>
+      <c r="G45" s="17" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="18.5">
@@ -1686,13 +1694,13 @@
         <v>0</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F46" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G46" s="18" t="s">
-        <v>111</v>
+        <v>33</v>
+      </c>
+      <c r="G46" s="17" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="14.5">
@@ -1713,13 +1721,13 @@
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
       <c r="D48" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G48" s="8"/>
     </row>
@@ -1730,13 +1738,13 @@
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
       <c r="D49" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F49" s="13" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G49" s="8"/>
     </row>
@@ -1769,13 +1777,13 @@
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
       <c r="D52" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F52" s="13" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G52" s="8"/>
     </row>
@@ -1786,13 +1794,13 @@
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
       <c r="D53" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F53" s="15" t="s">
-        <v>55</v>
+        <v>104</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="G53" s="8"/>
     </row>
@@ -1803,13 +1811,13 @@
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
       <c r="D54" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
       <c r="F54" s="13" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G54" s="8"/>
     </row>
@@ -1818,19 +1826,19 @@
         <v>53</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="F55" s="13" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G55" s="8"/>
     </row>
@@ -1839,19 +1847,19 @@
         <v>54</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="F56" s="13" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G56" s="8"/>
     </row>
@@ -1860,19 +1868,19 @@
         <v>55</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="F57" s="13" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G57" s="8"/>
     </row>
@@ -1905,13 +1913,13 @@
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E60" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E60" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="F60" s="13" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G60" s="8"/>
     </row>
@@ -1920,19 +1928,19 @@
         <v>59</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G61" s="8"/>
     </row>
@@ -1941,19 +1949,19 @@
         <v>60</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G62" s="8"/>
     </row>
@@ -1962,19 +1970,19 @@
         <v>61</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F63" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G63" s="8"/>
     </row>
@@ -1983,19 +1991,19 @@
         <v>62</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F64" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G64" s="8"/>
     </row>
@@ -2004,19 +2012,19 @@
         <v>63</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F65" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G65" s="8"/>
     </row>
@@ -2025,19 +2033,19 @@
         <v>64</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F66" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G66" s="8"/>
     </row>
@@ -2046,19 +2054,19 @@
         <v>65</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F67" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G67" s="8"/>
     </row>
@@ -2067,19 +2075,19 @@
         <v>66</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F68" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G68" s="8"/>
     </row>
@@ -2088,19 +2096,19 @@
         <v>67</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F69" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G69" s="8"/>
     </row>
@@ -2109,19 +2117,19 @@
         <v>68</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F70" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G70" s="8"/>
     </row>
@@ -2141,19 +2149,19 @@
         <v>70</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F72" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G72" s="8"/>
     </row>
@@ -2162,19 +2170,19 @@
         <v>71</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F73" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G73" s="8"/>
     </row>
@@ -2183,19 +2191,19 @@
         <v>72</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F74" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G74" s="8"/>
     </row>
@@ -2204,19 +2212,19 @@
         <v>73</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F75" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G75" s="8"/>
     </row>
@@ -2225,19 +2233,19 @@
         <v>74</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F76" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G76" s="8"/>
     </row>
@@ -2246,19 +2254,19 @@
         <v>75</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F77" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G77" s="8"/>
     </row>
@@ -2267,19 +2275,19 @@
         <v>76</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F78" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G78" s="8"/>
     </row>
@@ -2288,19 +2296,19 @@
         <v>77</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F79" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G79" s="8"/>
     </row>
@@ -2309,19 +2317,19 @@
         <v>78</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F80" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G80" s="8"/>
     </row>
@@ -2330,19 +2338,19 @@
         <v>79</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F81" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G81" s="8"/>
     </row>
@@ -2351,19 +2359,19 @@
         <v>80</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F82" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G82" s="8"/>
     </row>
@@ -2372,19 +2380,19 @@
         <v>81</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F83" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G83" s="8"/>
     </row>
@@ -2393,19 +2401,19 @@
         <v>82</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F84" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G84" s="8"/>
     </row>
@@ -2414,19 +2422,19 @@
         <v>83</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F85" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G85" s="8"/>
     </row>
@@ -2457,19 +2465,19 @@
         <v>86</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F88" s="13" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="G88" s="8"/>
     </row>
@@ -2478,19 +2486,19 @@
         <v>87</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F89" s="13" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="G89" s="8"/>
     </row>
@@ -2499,19 +2507,19 @@
         <v>88</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F90" s="13" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="G90" s="8"/>
     </row>
@@ -2520,19 +2528,19 @@
         <v>89</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F91" s="13" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="G91" s="8"/>
     </row>
@@ -2541,19 +2549,19 @@
         <v>90</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F92" s="13" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="G92" s="8"/>
     </row>
@@ -2562,19 +2570,19 @@
         <v>91</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="G93" s="8"/>
     </row>
@@ -2583,19 +2591,19 @@
         <v>92</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F94" s="13" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="G94" s="8"/>
     </row>
@@ -2615,19 +2623,19 @@
         <v>94</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="F96" s="13" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G96" s="8"/>
     </row>
@@ -2636,19 +2644,19 @@
         <v>95</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="F97" s="13" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G97" s="8"/>
     </row>
@@ -2657,19 +2665,19 @@
         <v>96</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="F98" s="13" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G98" s="8"/>
     </row>
@@ -2678,19 +2686,19 @@
         <v>97</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="F99" s="13" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G99" s="8"/>
     </row>
@@ -2729,7 +2737,7 @@
       <c r="E102" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F102" s="16" t="s">
+      <c r="F102" s="15" t="s">
         <v>19</v>
       </c>
       <c r="G102" s="8"/>
@@ -2739,19 +2747,19 @@
         <v>101</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F103" s="12" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="G103" s="8"/>
     </row>
@@ -2760,19 +2768,19 @@
         <v>102</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F104" s="16" t="s">
-        <v>63</v>
+        <v>51</v>
+      </c>
+      <c r="F104" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="G104" s="8"/>
     </row>
@@ -2781,19 +2789,19 @@
         <v>103</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F105" s="12" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="G105" s="8"/>
     </row>
@@ -2802,19 +2810,19 @@
         <v>104</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F106" s="16" t="s">
-        <v>63</v>
+        <v>51</v>
+      </c>
+      <c r="F106" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="G106" s="8"/>
     </row>
@@ -2823,19 +2831,19 @@
         <v>105</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F107" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G107" s="8"/>
     </row>
@@ -2844,19 +2852,19 @@
         <v>106</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F108" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G108" s="8"/>
     </row>
@@ -2865,19 +2873,19 @@
         <v>107</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F109" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G109" s="8"/>
     </row>
@@ -2886,19 +2894,19 @@
         <v>108</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F110" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G110" s="8"/>
     </row>
@@ -2907,19 +2915,19 @@
         <v>109</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F111" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G111" s="8"/>
     </row>
@@ -2928,19 +2936,19 @@
         <v>110</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F112" s="16" t="s">
-        <v>61</v>
+        <v>49</v>
+      </c>
+      <c r="F112" s="15" t="s">
+        <v>49</v>
       </c>
       <c r="G112" s="8"/>
     </row>
@@ -2949,19 +2957,19 @@
         <v>111</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F113" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G113" s="8"/>
     </row>
@@ -2970,19 +2978,19 @@
         <v>112</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F114" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G114" s="8"/>
     </row>
@@ -2991,19 +2999,19 @@
         <v>113</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F115" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G115" s="8"/>
     </row>
@@ -3012,19 +3020,19 @@
         <v>114</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F116" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G116" s="8"/>
     </row>
@@ -3033,19 +3041,19 @@
         <v>115</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F117" s="12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G117" s="8"/>
     </row>
@@ -3054,10 +3062,10 @@
         <v>116</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>11</v>
@@ -3065,7 +3073,7 @@
       <c r="E118" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F118" s="16" t="s">
+      <c r="F118" s="15" t="s">
         <v>12</v>
       </c>
       <c r="G118" s="8"/>
@@ -3075,10 +3083,10 @@
         <v>117</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>11</v>
@@ -3096,13 +3104,13 @@
         <v>118</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E120" s="4" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="F120" s="13" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="14.5">
@@ -3110,13 +3118,13 @@
         <v>119</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E121" s="4" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="F121" s="13" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="14.5">
@@ -3124,10 +3132,10 @@
         <v>120</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="14.5">
@@ -3135,10 +3143,10 @@
         <v>121</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>